<commit_message>
changes up to 12.02
</commit_message>
<xml_diff>
--- a/Data/Building_profiles_income/Household_assignment_summary.xlsx
+++ b/Data/Building_profiles_income/Household_assignment_summary.xlsx
@@ -435,16 +435,16 @@
         <v>3</v>
       </c>
       <c r="C2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G2">
         <v>1</v>
@@ -464,16 +464,16 @@
         <v>2</v>
       </c>
       <c r="D3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E3">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F3">
         <v>1</v>
       </c>
       <c r="G3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H3">
         <v>3</v>
@@ -490,16 +490,16 @@
         <v>2</v>
       </c>
       <c r="D4">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E4">
         <v>3</v>
       </c>
       <c r="F4">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="G4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H4">
         <v>3</v>
@@ -513,22 +513,22 @@
         <v>98</v>
       </c>
       <c r="C5">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D5">
         <v>2</v>
       </c>
       <c r="E5">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F5">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="G5">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H5">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -539,7 +539,7 @@
         <v>116</v>
       </c>
       <c r="C6">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D6">
         <v>1</v>
@@ -548,13 +548,13 @@
         <v>8</v>
       </c>
       <c r="F6">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G6">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="H6">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -565,22 +565,22 @@
         <v>120</v>
       </c>
       <c r="C7">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E7">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="F7">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="G7">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="H7">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -591,22 +591,22 @@
         <v>132</v>
       </c>
       <c r="C8">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D8">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E8">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F8">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G8">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="H8">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -620,13 +620,13 @@
         <v>10</v>
       </c>
       <c r="D9">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E9">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="F9">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G9">
         <v>16</v>
@@ -643,22 +643,22 @@
         <v>12</v>
       </c>
       <c r="C10">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E10">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F10">
         <v>0</v>
       </c>
       <c r="G10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H10">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -672,19 +672,19 @@
         <v>0</v>
       </c>
       <c r="D11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E11">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F11">
         <v>0</v>
       </c>
       <c r="G11">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H11">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:8">
@@ -695,13 +695,13 @@
         <v>15</v>
       </c>
       <c r="C12">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D12">
         <v>0</v>
       </c>
       <c r="E12">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F12">
         <v>0</v>
@@ -710,7 +710,7 @@
         <v>3</v>
       </c>
       <c r="H12">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:8">
@@ -721,22 +721,22 @@
         <v>16</v>
       </c>
       <c r="C13">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E13">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F13">
         <v>1</v>
       </c>
       <c r="G13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H13">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="14" spans="1:8">
@@ -747,19 +747,19 @@
         <v>17</v>
       </c>
       <c r="C14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E14">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F14">
         <v>0</v>
       </c>
       <c r="G14">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H14">
         <v>1</v>
@@ -773,19 +773,19 @@
         <v>21</v>
       </c>
       <c r="C15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E15">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="F15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G15">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H15">
         <v>0</v>
@@ -799,7 +799,7 @@
         <v>22</v>
       </c>
       <c r="C16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D16">
         <v>1</v>
@@ -808,13 +808,13 @@
         <v>3</v>
       </c>
       <c r="F16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G16">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H16">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:8">
@@ -831,13 +831,13 @@
         <v>0</v>
       </c>
       <c r="E17">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F17">
         <v>0</v>
       </c>
       <c r="G17">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H17">
         <v>2</v>
@@ -851,22 +851,22 @@
         <v>24</v>
       </c>
       <c r="C18">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D18">
         <v>0</v>
       </c>
       <c r="E18">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F18">
         <v>0</v>
       </c>
       <c r="G18">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H18">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="19" spans="1:8">
@@ -880,19 +880,19 @@
         <v>1</v>
       </c>
       <c r="D19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E19">
         <v>1</v>
       </c>
       <c r="F19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G19">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H19">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:8">
@@ -903,22 +903,22 @@
         <v>26</v>
       </c>
       <c r="C20">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E20">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F20">
         <v>1</v>
       </c>
       <c r="G20">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H20">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="21" spans="1:8">
@@ -929,22 +929,22 @@
         <v>52</v>
       </c>
       <c r="C21">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E21">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F21">
         <v>0</v>
       </c>
       <c r="G21">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H21">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="22" spans="1:8">
@@ -955,19 +955,19 @@
         <v>53</v>
       </c>
       <c r="C22">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D22">
         <v>0</v>
       </c>
       <c r="E22">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F22">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G22">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H22">
         <v>4</v>
@@ -981,22 +981,22 @@
         <v>54</v>
       </c>
       <c r="C23">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D23">
         <v>1</v>
       </c>
       <c r="E23">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="F23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G23">
         <v>4</v>
       </c>
       <c r="H23">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:8">
@@ -1007,22 +1007,22 @@
         <v>55</v>
       </c>
       <c r="C24">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F24">
         <v>1</v>
       </c>
       <c r="G24">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H24">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="25" spans="1:8">
@@ -1033,22 +1033,22 @@
         <v>85</v>
       </c>
       <c r="C25">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D25">
         <v>2</v>
       </c>
       <c r="E25">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F25">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G25">
+        <v>5</v>
+      </c>
+      <c r="H25">
         <v>11</v>
-      </c>
-      <c r="H25">
-        <v>9</v>
       </c>
     </row>
     <row r="26" spans="1:8">
@@ -1059,7 +1059,7 @@
         <v>86</v>
       </c>
       <c r="C26">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D26">
         <v>0</v>
@@ -1068,10 +1068,10 @@
         <v>2</v>
       </c>
       <c r="F26">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G26">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="H26">
         <v>4</v>
@@ -1085,22 +1085,22 @@
         <v>87</v>
       </c>
       <c r="C27">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D27">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E27">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F27">
         <v>1</v>
       </c>
       <c r="G27">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H27">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="28" spans="1:8">
@@ -1117,16 +1117,16 @@
         <v>1</v>
       </c>
       <c r="E28">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F28">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G28">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="H28">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="29" spans="1:8">
@@ -1143,16 +1143,16 @@
         <v>1</v>
       </c>
       <c r="E29">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="F29">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G29">
         <v>3</v>
       </c>
       <c r="H29">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="30" spans="1:8">
@@ -1163,22 +1163,22 @@
         <v>100</v>
       </c>
       <c r="C30">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D30">
         <v>0</v>
       </c>
       <c r="E30">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F30">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G30">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="H30">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="31" spans="1:8">
@@ -1192,19 +1192,19 @@
         <v>0</v>
       </c>
       <c r="D31">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E31">
         <v>4</v>
       </c>
       <c r="F31">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G31">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H31">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="32" spans="1:8">
@@ -1215,22 +1215,22 @@
         <v>102</v>
       </c>
       <c r="C32">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D32">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E32">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="F32">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G32">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H32">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="33" spans="1:8">
@@ -1241,22 +1241,22 @@
         <v>103</v>
       </c>
       <c r="C33">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="D33">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E33">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F33">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G33">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H33">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="34" spans="1:8">
@@ -1270,19 +1270,19 @@
         <v>3</v>
       </c>
       <c r="D34">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E34">
         <v>2</v>
       </c>
       <c r="F34">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G34">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H34">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="35" spans="1:8">
@@ -1293,22 +1293,22 @@
         <v>105</v>
       </c>
       <c r="C35">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D35">
         <v>0</v>
       </c>
       <c r="E35">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F35">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G35">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="H35">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="36" spans="1:8">
@@ -1319,22 +1319,22 @@
         <v>108</v>
       </c>
       <c r="C36">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D36">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E36">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F36">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G36">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H36">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="37" spans="1:8">
@@ -1348,19 +1348,19 @@
         <v>2</v>
       </c>
       <c r="D37">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E37">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F37">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G37">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H37">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="38" spans="1:8">
@@ -1371,22 +1371,22 @@
         <v>57</v>
       </c>
       <c r="C38">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D38">
         <v>0</v>
       </c>
       <c r="E38">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F38">
         <v>2</v>
       </c>
       <c r="G38">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H38">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="39" spans="1:8">
@@ -1397,19 +1397,19 @@
         <v>58</v>
       </c>
       <c r="C39">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D39">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E39">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F39">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G39">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H39">
         <v>5</v>
@@ -1423,22 +1423,22 @@
         <v>59</v>
       </c>
       <c r="C40">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D40">
         <v>0</v>
       </c>
       <c r="E40">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F40">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G40">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H40">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="41" spans="1:8">
@@ -1449,22 +1449,22 @@
         <v>60</v>
       </c>
       <c r="C41">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D41">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E41">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F41">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G41">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H41">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="42" spans="1:8">
@@ -1475,13 +1475,13 @@
         <v>61</v>
       </c>
       <c r="C42">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D42">
         <v>0</v>
       </c>
       <c r="E42">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F42">
         <v>0</v>
@@ -1490,7 +1490,7 @@
         <v>6</v>
       </c>
       <c r="H42">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="43" spans="1:8">
@@ -1501,7 +1501,7 @@
         <v>62</v>
       </c>
       <c r="C43">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D43">
         <v>0</v>
@@ -1510,10 +1510,10 @@
         <v>2</v>
       </c>
       <c r="F43">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G43">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H43">
         <v>3</v>
@@ -1536,13 +1536,13 @@
         <v>1</v>
       </c>
       <c r="F44">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G44">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H44">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="45" spans="1:8">
@@ -1553,22 +1553,22 @@
         <v>66</v>
       </c>
       <c r="C45">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D45">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E45">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F45">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="G45">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H45">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="46" spans="1:8">
@@ -1579,22 +1579,22 @@
         <v>90</v>
       </c>
       <c r="C46">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D46">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E46">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F46">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G46">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H46">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="47" spans="1:8">
@@ -1605,22 +1605,22 @@
         <v>91</v>
       </c>
       <c r="C47">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D47">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E47">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F47">
         <v>1</v>
       </c>
       <c r="G47">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H47">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="48" spans="1:8">
@@ -1631,22 +1631,22 @@
         <v>92</v>
       </c>
       <c r="C48">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D48">
         <v>0</v>
       </c>
       <c r="E48">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F48">
         <v>1</v>
       </c>
       <c r="G48">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H48">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="49" spans="1:8">
@@ -1657,22 +1657,22 @@
         <v>99</v>
       </c>
       <c r="C49">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D49">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E49">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F49">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G49">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H49">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="50" spans="1:8">
@@ -1686,19 +1686,19 @@
         <v>1</v>
       </c>
       <c r="D50">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E50">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F50">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G50">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H50">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="51" spans="1:8">
@@ -1709,22 +1709,22 @@
         <v>112</v>
       </c>
       <c r="C51">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D51">
         <v>0</v>
       </c>
       <c r="E51">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F51">
         <v>0</v>
       </c>
       <c r="G51">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H51">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="52" spans="1:8">
@@ -1738,7 +1738,7 @@
         <v>2</v>
       </c>
       <c r="D52">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E52">
         <v>3</v>
@@ -1747,10 +1747,10 @@
         <v>1</v>
       </c>
       <c r="G52">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H52">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="53" spans="1:8">
@@ -1764,19 +1764,19 @@
         <v>1</v>
       </c>
       <c r="D53">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E53">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F53">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G53">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="H53">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="54" spans="1:8">
@@ -1787,22 +1787,22 @@
         <v>124</v>
       </c>
       <c r="C54">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D54">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E54">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F54">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G54">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H54">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="55" spans="1:8">
@@ -1813,22 +1813,22 @@
         <v>126</v>
       </c>
       <c r="C55">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D55">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E55">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F55">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G55">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H55">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="56" spans="1:8">
@@ -1839,22 +1839,22 @@
         <v>127</v>
       </c>
       <c r="C56">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D56">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E56">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="F56">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G56">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H56">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="57" spans="1:8">
@@ -1865,7 +1865,7 @@
         <v>128</v>
       </c>
       <c r="C57">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D57">
         <v>0</v>
@@ -1877,7 +1877,7 @@
         <v>0</v>
       </c>
       <c r="G57">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H57">
         <v>2</v>
@@ -1891,19 +1891,19 @@
         <v>136</v>
       </c>
       <c r="C58">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D58">
         <v>1</v>
       </c>
       <c r="E58">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F58">
         <v>1</v>
       </c>
       <c r="G58">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="H58">
         <v>5</v>
@@ -1920,19 +1920,19 @@
         <v>3</v>
       </c>
       <c r="D59">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E59">
         <v>5</v>
       </c>
       <c r="F59">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G59">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="H59">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="60" spans="1:8">
@@ -1949,16 +1949,16 @@
         <v>0</v>
       </c>
       <c r="E60">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F60">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G60">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H60">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="61" spans="1:8">
@@ -1972,7 +1972,7 @@
         <v>0</v>
       </c>
       <c r="D61">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E61">
         <v>1</v>
@@ -1981,10 +1981,10 @@
         <v>0</v>
       </c>
       <c r="G61">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H61">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="62" spans="1:8">
@@ -1995,22 +1995,22 @@
         <v>69</v>
       </c>
       <c r="C62">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D62">
         <v>0</v>
       </c>
       <c r="E62">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F62">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G62">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H62">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="63" spans="1:8">
@@ -2027,16 +2027,16 @@
         <v>0</v>
       </c>
       <c r="E63">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F63">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G63">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H63">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="64" spans="1:8">
@@ -2053,16 +2053,16 @@
         <v>0</v>
       </c>
       <c r="E64">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F64">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G64">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H64">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="65" spans="1:8">
@@ -2073,7 +2073,7 @@
         <v>81</v>
       </c>
       <c r="C65">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D65">
         <v>0</v>
@@ -2082,7 +2082,7 @@
         <v>2</v>
       </c>
       <c r="F65">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G65">
         <v>2</v>
@@ -2099,22 +2099,22 @@
         <v>82</v>
       </c>
       <c r="C66">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D66">
         <v>0</v>
       </c>
       <c r="E66">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F66">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G66">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H66">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="67" spans="1:8">
@@ -2128,19 +2128,19 @@
         <v>1</v>
       </c>
       <c r="D67">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E67">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F67">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G67">
         <v>3</v>
       </c>
       <c r="H67">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="68" spans="1:8">
@@ -2154,19 +2154,19 @@
         <v>2</v>
       </c>
       <c r="D68">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E68">
         <v>2</v>
       </c>
       <c r="F68">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G68">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H68">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="69" spans="1:8">
@@ -2180,19 +2180,19 @@
         <v>4</v>
       </c>
       <c r="D69">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E69">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F69">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G69">
         <v>4</v>
       </c>
       <c r="H69">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="70" spans="1:8">
@@ -2203,22 +2203,22 @@
         <v>134</v>
       </c>
       <c r="C70">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D70">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E70">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="F70">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G70">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="H70">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="71" spans="1:8">
@@ -2235,16 +2235,16 @@
         <v>1</v>
       </c>
       <c r="E71">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F71">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G71">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H71">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="72" spans="1:8">
@@ -2255,22 +2255,22 @@
         <v>41</v>
       </c>
       <c r="C72">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D72">
         <v>0</v>
       </c>
       <c r="E72">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F72">
         <v>0</v>
       </c>
       <c r="G72">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H72">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="73" spans="1:8">
@@ -2281,10 +2281,10 @@
         <v>42</v>
       </c>
       <c r="C73">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D73">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E73">
         <v>2</v>
@@ -2293,10 +2293,10 @@
         <v>0</v>
       </c>
       <c r="G73">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H73">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="74" spans="1:8">
@@ -2307,22 +2307,22 @@
         <v>43</v>
       </c>
       <c r="C74">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D74">
         <v>0</v>
       </c>
       <c r="E74">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F74">
         <v>0</v>
       </c>
       <c r="G74">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H74">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="75" spans="1:8">
@@ -2333,22 +2333,22 @@
         <v>44</v>
       </c>
       <c r="C75">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D75">
         <v>0</v>
       </c>
       <c r="E75">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F75">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G75">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H75">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="76" spans="1:8">
@@ -2362,19 +2362,19 @@
         <v>1</v>
       </c>
       <c r="D76">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E76">
         <v>1</v>
       </c>
       <c r="F76">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G76">
         <v>0</v>
       </c>
       <c r="H76">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="77" spans="1:8">
@@ -2385,22 +2385,22 @@
         <v>46</v>
       </c>
       <c r="C77">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D77">
         <v>0</v>
       </c>
       <c r="E77">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F77">
         <v>0</v>
       </c>
       <c r="G77">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H77">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="78" spans="1:8">
@@ -2411,22 +2411,22 @@
         <v>47</v>
       </c>
       <c r="C78">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D78">
         <v>0</v>
       </c>
       <c r="E78">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F78">
         <v>0</v>
       </c>
       <c r="G78">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H78">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="79" spans="1:8">
@@ -2437,13 +2437,13 @@
         <v>48</v>
       </c>
       <c r="C79">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D79">
         <v>0</v>
       </c>
       <c r="E79">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F79">
         <v>1</v>
@@ -2452,7 +2452,7 @@
         <v>2</v>
       </c>
       <c r="H79">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="80" spans="1:8">
@@ -2463,13 +2463,13 @@
         <v>70</v>
       </c>
       <c r="C80">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D80">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E80">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F80">
         <v>1</v>
@@ -2489,22 +2489,22 @@
         <v>72</v>
       </c>
       <c r="C81">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D81">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E81">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F81">
         <v>0</v>
       </c>
       <c r="G81">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H81">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="82" spans="1:8">
@@ -2515,16 +2515,16 @@
         <v>73</v>
       </c>
       <c r="C82">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D82">
         <v>0</v>
       </c>
       <c r="E82">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F82">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G82">
         <v>3</v>
@@ -2547,16 +2547,16 @@
         <v>0</v>
       </c>
       <c r="E83">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F83">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G83">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H83">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="84" spans="1:8">
@@ -2570,19 +2570,19 @@
         <v>1</v>
       </c>
       <c r="D84">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E84">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F84">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G84">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H84">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="85" spans="1:8">
@@ -2593,13 +2593,13 @@
         <v>76</v>
       </c>
       <c r="C85">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D85">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E85">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F85">
         <v>0</v>
@@ -2608,7 +2608,7 @@
         <v>1</v>
       </c>
       <c r="H85">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="86" spans="1:8">
@@ -2619,19 +2619,19 @@
         <v>83</v>
       </c>
       <c r="C86">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D86">
         <v>1</v>
       </c>
       <c r="E86">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F86">
         <v>1</v>
       </c>
       <c r="G86">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H86">
         <v>3</v>
@@ -2651,16 +2651,16 @@
         <v>0</v>
       </c>
       <c r="E87">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F87">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G87">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H87">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="88" spans="1:8">
@@ -2671,22 +2671,22 @@
         <v>93</v>
       </c>
       <c r="C88">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D88">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E88">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F88">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G88">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="H88">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="89" spans="1:8">
@@ -2700,19 +2700,19 @@
         <v>2</v>
       </c>
       <c r="D89">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E89">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F89">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G89">
         <v>3</v>
       </c>
       <c r="H89">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="90" spans="1:8">
@@ -2723,22 +2723,22 @@
         <v>95</v>
       </c>
       <c r="C90">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D90">
         <v>1</v>
       </c>
       <c r="E90">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="F90">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G90">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H90">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="91" spans="1:8">
@@ -2749,22 +2749,22 @@
         <v>96</v>
       </c>
       <c r="C91">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D91">
         <v>1</v>
       </c>
       <c r="E91">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F91">
         <v>1</v>
       </c>
       <c r="G91">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H91">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="92" spans="1:8">
@@ -2775,22 +2775,22 @@
         <v>97</v>
       </c>
       <c r="C92">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D92">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E92">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F92">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G92">
         <v>4</v>
       </c>
       <c r="H92">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="93" spans="1:8">
@@ -2801,22 +2801,22 @@
         <v>117</v>
       </c>
       <c r="C93">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D93">
         <v>1</v>
       </c>
       <c r="E93">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F93">
         <v>1</v>
       </c>
       <c r="G93">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H93">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="94" spans="1:8">
@@ -2827,19 +2827,19 @@
         <v>121</v>
       </c>
       <c r="C94">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D94">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E94">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F94">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G94">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="H94">
         <v>6</v>
@@ -2853,22 +2853,22 @@
         <v>122</v>
       </c>
       <c r="C95">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D95">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E95">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F95">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="G95">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="H95">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="96" spans="1:8">
@@ -2879,19 +2879,19 @@
         <v>123</v>
       </c>
       <c r="C96">
+        <v>3</v>
+      </c>
+      <c r="D96">
+        <v>2</v>
+      </c>
+      <c r="E96">
         <v>6</v>
       </c>
-      <c r="D96">
-        <v>0</v>
-      </c>
-      <c r="E96">
-        <v>4</v>
-      </c>
       <c r="F96">
         <v>4</v>
       </c>
       <c r="G96">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H96">
         <v>5</v>
@@ -2905,22 +2905,22 @@
         <v>129</v>
       </c>
       <c r="C97">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D97">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E97">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F97">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G97">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="H97">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="98" spans="1:8">
@@ -2931,22 +2931,22 @@
         <v>130</v>
       </c>
       <c r="C98">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D98">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E98">
         <v>6</v>
       </c>
       <c r="F98">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G98">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="H98">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="99" spans="1:8">
@@ -2963,16 +2963,16 @@
         <v>0</v>
       </c>
       <c r="E99">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F99">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G99">
         <v>1</v>
       </c>
       <c r="H99">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="100" spans="1:8">
@@ -2983,19 +2983,19 @@
         <v>29</v>
       </c>
       <c r="C100">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D100">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E100">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F100">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G100">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="H100">
         <v>1</v>
@@ -3009,7 +3009,7 @@
         <v>30</v>
       </c>
       <c r="C101">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D101">
         <v>1</v>
@@ -3018,13 +3018,13 @@
         <v>5</v>
       </c>
       <c r="F101">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G101">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H101">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="102" spans="1:8">
@@ -3035,22 +3035,22 @@
         <v>31</v>
       </c>
       <c r="C102">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D102">
         <v>0</v>
       </c>
       <c r="E102">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="F102">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G102">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H102">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="103" spans="1:8">
@@ -3067,13 +3067,13 @@
         <v>1</v>
       </c>
       <c r="E103">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F103">
         <v>3</v>
       </c>
       <c r="G103">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H103">
         <v>3</v>
@@ -3087,19 +3087,19 @@
         <v>33</v>
       </c>
       <c r="C104">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D104">
         <v>0</v>
       </c>
       <c r="E104">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F104">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G104">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="H104">
         <v>2</v>
@@ -3113,22 +3113,22 @@
         <v>34</v>
       </c>
       <c r="C105">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D105">
         <v>1</v>
       </c>
       <c r="E105">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F105">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G105">
         <v>2</v>
       </c>
       <c r="H105">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="106" spans="1:8">
@@ -3139,22 +3139,22 @@
         <v>36</v>
       </c>
       <c r="C106">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D106">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E106">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F106">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G106">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="H106">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="107" spans="1:8">
@@ -3165,22 +3165,22 @@
         <v>37</v>
       </c>
       <c r="C107">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D107">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E107">
         <v>2</v>
       </c>
       <c r="F107">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G107">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H107">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="108" spans="1:8">
@@ -3191,19 +3191,19 @@
         <v>38</v>
       </c>
       <c r="C108">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D108">
         <v>0</v>
       </c>
       <c r="E108">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F108">
         <v>2</v>
       </c>
       <c r="G108">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H108">
         <v>2</v>
@@ -3217,22 +3217,22 @@
         <v>39</v>
       </c>
       <c r="C109">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D109">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E109">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F109">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G109">
         <v>5</v>
       </c>
       <c r="H109">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="110" spans="1:8">
@@ -3243,22 +3243,22 @@
         <v>40</v>
       </c>
       <c r="C110">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D110">
         <v>2</v>
       </c>
       <c r="E110">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F110">
         <v>4</v>
       </c>
       <c r="G110">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="H110">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>